<commit_message>
Fall Off Report Updated - PS: if DateOFSale is NULL, that Debi-Check will not be pulled
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateFallOffReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateFallOffReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2452B7-A1B7-4CF7-9562-ACBE6E193D11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EB7661-D910-4395-A363-131DBC3698EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="CancellationsDatasheet" sheetId="3" r:id="rId3"/>
     <sheet name="CarriedForwardDatasheet" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -463,6 +463,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,12 +548,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -915,34 +915,34 @@
     <row r="1" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34" t="s">
+      <c r="M1" s="35"/>
+      <c r="N1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="29" t="s">
+      <c r="Q1" s="39"/>
+      <c r="R1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="29"/>
+      <c r="S1" s="31"/>
     </row>
     <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,57 +1037,58 @@
     <col min="8" max="8" width="11.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="5"/>
     <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
-    <col min="11" max="19" width="9.140625" style="5"/>
-    <col min="20" max="20" width="9.140625" style="23"/>
-    <col min="21" max="21" width="9.140625" style="5"/>
-    <col min="22" max="22" width="11" style="3" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" style="5" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="14" max="21" width="9.140625" style="5"/>
+    <col min="22" max="22" width="9.140625" style="23"/>
+    <col min="23" max="23" width="9.140625" style="5"/>
+    <col min="24" max="24" width="11" style="3" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="17" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="40"/>
+      <c r="N1" s="44" t="s">
         <v>8</v>
-      </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44" t="s">
-        <v>9</v>
       </c>
       <c r="O1" s="45"/>
       <c r="P1" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="50"/>
-      <c r="V1" s="41" t="s">
+      <c r="W1" s="52"/>
+      <c r="X1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="41"/>
-      <c r="X1" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y1" s="38"/>
+      <c r="Y1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="17" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -1123,10 +1124,10 @@
       <c r="K2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="20" t="s">
         <v>2</v>
       </c>
       <c r="N2" s="21" t="s">
@@ -1142,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S2" s="22" t="s">
         <v>2</v>
@@ -1150,13 +1151,13 @@
       <c r="T2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="W2" s="20" t="s">
+      <c r="U2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="24" t="s">
         <v>2</v>
       </c>
       <c r="X2" s="19" t="s">
@@ -1178,8 +1179,8 @@
       <c r="I3" s="26"/>
       <c r="J3" s="25"/>
       <c r="K3" s="26"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="26"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="29"/>
       <c r="N3" s="27"/>
       <c r="O3" s="26"/>
       <c r="P3" s="27"/>
@@ -1188,28 +1189,28 @@
       <c r="S3" s="26"/>
       <c r="T3" s="27"/>
       <c r="U3" s="26"/>
-      <c r="V3" s="25"/>
+      <c r="V3" s="27"/>
       <c r="W3" s="26"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="56"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="26"/>
       <c r="Z3" s="28"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L4" s="23"/>
       <c r="N4" s="23"/>
       <c r="P4" s="23"/>
       <c r="R4" s="23"/>
+      <c r="T4" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:W1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1241,18 +1242,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1333,19 +1334,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">

</xml_diff>